<commit_message>
Atualizando calendário de 2023-24
</commit_message>
<xml_diff>
--- a/calendario-jumper.xlsx
+++ b/calendario-jumper.xlsx
@@ -1,477 +1,431 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Downloads\twitterBot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Downloads\Projetos\twitterBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C947636C-54B3-4911-839B-1056C2870477}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD96264-40E7-4A39-B084-69A35ABF416F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="149">
-  <si>
-    <t>18/10/22 (terça-feira): Philadelphia 76ers x Boston Celtics (Amazon Prime Video – 20h30) / Los Angeles Lakers x Golden State Warriors (Amazon Prime Video – 23h)</t>
-  </si>
-  <si>
-    <t>19/10/22 (quarta-feira): New York Knicks x Memphis Grizzlies (ESPN 2 – 20h30) / Dallas Mavericks x Phoenix Suns (ESPN 2 – 23h)</t>
-  </si>
-  <si>
-    <t>20/10/22 (quinta-feira): Milwaukee Bucks x Philadelphia 76ers (Amazon Prime Video – 20h30) / Los Angeles Clippers x Los Angeles Lakers (Amazon Prime Video – 23h)</t>
-  </si>
-  <si>
-    <t>21/10/22 (sexta-feira): Boston Celtics x Miami Heat (ESPN 2 – 20h30) / Denver Nuggets x Golden State Warriors (ESPN 2 – 23h)</t>
-  </si>
-  <si>
-    <t>22/10/22 (sábado): Memphis Grizzlies x Dallas Mavericks (ESPN 2 – 21h30)</t>
-  </si>
-  <si>
-    <t>23/10/22 (domingo): Phoenix Suns x Los Angeles Clippers (TNT / SporTV 2 / Gaules / Facebook da CNN Brasil – 23h)</t>
-  </si>
-  <si>
-    <t>24/10/22 (segunda-feira): Denver Nuggets x Portland Trail Blazers (Band / TNT / SporTV 2/ Gaules / Facebook da CNN Brasil – 23h)</t>
-  </si>
-  <si>
-    <t>25/10/22 (terça-feira): Dallas Mavericks x New Orleans Pelicans (Amazon Prime Video – 20h30) / Golden State Warriors x Phoenix Suns (Amazon Prime Video – 23h)</t>
-  </si>
-  <si>
-    <t>26/10/22 (quarta-feira): Brooklyn Nets x Milwaukee Bucks (ESPN 2 – 20h30) / Los Angeles Lakers x Denver Nuggets (ESPN 2 – 23h)</t>
-  </si>
-  <si>
-    <t>28/10/22 (sexta-feira): Indiana Pacers x Washington Wizards (ESPN 2 – 20h30) / New Orleans Pelicans x Phoenix Suns (ESPN 2 – 23h)</t>
-  </si>
-  <si>
-    <t>29/10/22 (sábado): Memphis Grizzlies x Utah Jazz (ESPN 2 – 22h)</t>
-  </si>
-  <si>
-    <t>30/10/22 (domingo): Denver Nuggets x Los Angeles Lakers (TNT / SporTV 2 / Gaules / Facebook da CNN Brasil – 22h30)</t>
-  </si>
-  <si>
-    <t>31/10/22 (segunda-feira): Houston Rockets x Los Angeles Clippers (Band / TNT / SporTV 2/ Gaules / Facebook da CNN Brasil – 23h30)</t>
-  </si>
-  <si>
-    <t>01/11/22 (terça-feira): Orlando Magic x Oklahoma City Thunder (Amazon Prime Video – 20h30) / Minnesota Timberwolves x Phoenix Suns (Amazon Prime Video – 23h)</t>
-  </si>
-  <si>
-    <t>02/11/22 (quarta-feira): Boston Celtics x Cleveland Cavaliers (ESPN 2 – 20h30) / Memphis Grizzlies x Portland Trail Blazers (ESPN 2 – 23h)</t>
-  </si>
-  <si>
-    <t>04/11/22 (sexta-feira): Chicago Bulls x Boston Celtics (ESPN 2 – 20h30) / Milwaukee Bucks x Minnesota Timberwolves (ESPN 2 – 23h)</t>
-  </si>
-  <si>
-    <t>05/11/22 (sábado): Boston Celtics x New York Knicks (ESPN 2 – 20h30)</t>
-  </si>
-  <si>
-    <t>06/11/22 (domingo): Cleveland Cavaliers x Los Angeles Lakers (TNT / SporTV 2 / Gaules / Facebook da CNN Brasil – 17h30)</t>
-  </si>
-  <si>
-    <t>07/11/22 (segunda-feira): Sacramento Kings x Golden State Warriors (Band / TNT / SporTV 2 / Gaules / Facebook da CNN Brasil – 0h)</t>
-  </si>
-  <si>
-    <t>09/11/22 (quarta-feira): New York Knicks x Brooklyn Nets (ESPN 2 – 21h30) / Los Angeles Lakers x Los Angeles Clippers (ESPN 2 – 0h)</t>
-  </si>
-  <si>
-    <t>10/11/22 (quinta-feira): Philadelphia 76ers x Atlanta Hawks (Amazon Prime Video – 21h30)</t>
-  </si>
-  <si>
-    <t>11/11/22 (sexta-feira): Minnesota Timberwolves x Memphis Grizzlies (ESPN 2 – 23h30)</t>
-  </si>
-  <si>
-    <t>12/11/22 (sábado): Atlanta Hawks x Philadelphia 76ers (ESPN 2 – 21h30)</t>
-  </si>
-  <si>
-    <t>13/11/22 (domingo): Brooklyn Nets x Los Angeles Lakers (Band / TNT / SporTV 2 / Gaules / Facebook da CNN Brasil – 23h30)</t>
-  </si>
-  <si>
-    <t>14/11/22 (segunda-feira): San Antonio Spurs x Golden State Warriors (Band / TNT / SporTV 2 / Gaules / Facebook da CNN Brasil – 0h)</t>
-  </si>
-  <si>
-    <t>15/11/22 (terça-feira): Memphis Grizzlies x New Orleans Pelicans (Amazon Prime Video – 21h30) / New York Knicks x Utah Jazz (Amazon Prime Video – 0h)</t>
-  </si>
-  <si>
-    <t>16/11/22 (quarta-feira): Boston Celtics x Atlanta Hawks (ESPN 2 – 21h30) / Golden State Warriors x Phoenix Suns (ESPN 2 – 0h)</t>
-  </si>
-  <si>
-    <t>18/11/22 (sexta-feira): Milwaukee Bucks x Philadelphia 76ers (ESPN 2 – 21h30) / New York Knicks x Golden State Warriors (ESPN 2 – 0h)</t>
-  </si>
-  <si>
-    <t>19/11/22 (sábado): Utah Jazz x Portland Trail Blazers (ESPN 2 – 0h)</t>
-  </si>
-  <si>
-    <t>21/11/22 (segunda-feira): Utah Jazz x Los Angeles Clippers (Band / TNT / SporTV 2 / Gaules / Facebook da CNN Brasil – 0h30)</t>
-  </si>
-  <si>
-    <t>22/11/22 (terça-feira): Brooklyn Nets x Philadelphia 76ers (Amazon Prime Video – 21h30) / Los Angeles Lakers x Phoenix Suns (Amazon Prime Video – 0h)</t>
-  </si>
-  <si>
-    <t>23/11/22 (quarta-feira): Dallas Mavericks x Boston Celtics (ESPN 2 – 21h30) / Los Angeles Clippers x Golden State Warriors (ESPN 2 – 0h)</t>
-  </si>
-  <si>
-    <t>25/11/22 (sexta-feira): Utah Jazz x Golden State Warriors (ESPN 2 – 0h)</t>
-  </si>
-  <si>
-    <t>26/11/22 (sábado): Los Angeles Lakers x San Antonio Spurs (ESPN 2 – 22h)</t>
-  </si>
-  <si>
-    <t>27/11/22 (domingo): Dallas Mavericks x Milwaukee Bucks (TNT / SporTV 2 / Gaules / Facebook da CNN Brasil – 22h)</t>
-  </si>
-  <si>
-    <t>28/11/22 (segunda-feira): Indiana Pacers x Los Angeles Lakers (Band / TNT / SporTV 2 / Gaules / Facebook da CNN Brasil – 0h30)</t>
-  </si>
-  <si>
-    <t>29/11/22 (terça-feira): Golden State Warriors x Dallas Mavericks (Amazon Prime Video – 21h30) / Los Angeles Clippers x Portland Trail Blazers (Amazon Prime Video – 0h)</t>
-  </si>
-  <si>
-    <t>30/11/22 (quarta-feira): Chicago Bulls x Phoenix Suns (ESPN 2 – 23h)</t>
-  </si>
-  <si>
-    <t>02/12/22 (sexta-feira): Los Angeles Lakers x Milwaukee Bucks (ESPN 2 – 21h30) / Chicago Bulls x Golden State Warriors (ESPN 2 – 0h)</t>
-  </si>
-  <si>
-    <t>03/12/22 (sábado): Milwaukee Bucks x Charlotte Hornets (ESPN 2 – 20h)</t>
-  </si>
-  <si>
-    <t>04/12/22 (domingo): Boston Celtics x Brooklyn Nets (TNT / SporTV 2 / Gaules / Facebook da CNN Brasil – 20h)</t>
-  </si>
-  <si>
-    <t>05/12/22 (segunda-feira): Phoenix Suns x Dallas Mavericks (Band / TNT / SporTV 2 / Gaules / Facebook da CNN Brasil – 22h30)</t>
-  </si>
-  <si>
-    <t>06/12/22 (terça-feira): Los Angeles Lakers x Cleveland Cavaliers (Amazon Prime Video – 21h30) / Dallas Mavericks x Denver Nuggets (Amazon Prime Video – 0h)</t>
-  </si>
-  <si>
-    <t>07/12/22 (quarta-feira): Atlanta Hawks x New York Knicks (ESPN 2 – 21h30) / Boston Celtics x Phoenix Suns (ESPN 2 – 0h)</t>
-  </si>
-  <si>
-    <t>09/12/22 (sexta-feira): Los Angeles Lakers x Philadelphia 76ers (ESPN 2 – 21h30) / Milwaukee Bucks x Dallas Mavericks (ESPN 2 – 0h)</t>
-  </si>
-  <si>
-    <t>10/12/22 (sábado): Boston Celtics x Golden State Warriors (ESPN 2 – 22h30)</t>
-  </si>
-  <si>
-    <t>12/12/22 (segunda-feira): Boston Celtics x Los Angeles Clippers (Band / TNT / SporTV 2 / Gaules / Facebook da CNN Brasil – 0h30)</t>
-  </si>
-  <si>
-    <t>13/12/22 (terça-feira): Golden State Warriors x Milwaukee Bucks (Amazon Prime Video – 21h30) / Boston Celtics x Los Angeles Lakers (Amazon Prime Video – 0h)</t>
-  </si>
-  <si>
-    <t>14/12/22 (quarta-feira): New York Knicks x Chicago Bulls (ESPN 2 – 21h30) / Minnesota Timberwolves x Los Angeles Clippers (ESPN 2 – 0h)</t>
-  </si>
-  <si>
-    <t>16/12/22 (sexta-feira): Golden State Warriors x Philadelphia 76ers (ESPN 2 – 21h30) / Denver Nuggets x Los Angeles Lakers (ESPN 2 – 0h)</t>
-  </si>
-  <si>
-    <t>17/12/22 (sábado): Miami Heat x San Antonio Spurs (ESPN 2 – 19h)</t>
-  </si>
-  <si>
-    <t>18/12/22 (domingo): Washington Wizards x Los Angeles Lakers (Band / TNT / SporTV 2 / Gaules / Facebook da CNN Brasil – 23h30)</t>
-  </si>
-  <si>
-    <t>19/12/22 (segunda-feira): Los Angeles Lakers x Phoenix Suns (Band / TNT / SporTV 2 / Gaules / Facebook da CNN Brasil – 23h)</t>
-  </si>
-  <si>
-    <t>20/12/22 (terça-feira): Golden State Warriors x New York Knicks (Amazon Prime Video – 21h30) / Memphis Grizzlies x Denver Nuggets (Amazon Prime Video – 0h)</t>
-  </si>
-  <si>
-    <t>21/12/22 (quarta-feira): Golden State Warriors x Brooklyn Nets (ESPN 2 – 21h30)</t>
-  </si>
-  <si>
-    <t>23/12/22 (sexta-feira): Memphis Grizzlies x Phoenix Suns (ESPN 2 – 0h)</t>
-  </si>
-  <si>
-    <t>25/12/22 (domingo): Philadelphia 76ers x New York Knicks (ESPN 2 – 14h) / Los Angeles Lakers x Dallas Mavericks (ESPN 2 – 16h30) / Milwaukee Bucks x Boston Celtics (ESPN 2 – 19h) / Memphis Grizzlies x Golden State Warriors (ESPN 2 – 22h) / Phoenix Suns x Denver Nuggets (ESPN 2 – 0h30)</t>
-  </si>
-  <si>
-    <t>26/12/22 (segunda-feira): Charlotte Hornets x Portland Trail Blazers (Band / TNT / SporTV 2 / Gaules / Facebook da CNN Brasil – 0h)</t>
-  </si>
-  <si>
-    <t>27/12/22 (terça-feira): Los Angeles Clippers x Toronto Raptors (Amazon Prime Video – 21h30) / Charlote Hornets x Golden State Warriors (Amazon Prime Video – 0h)</t>
-  </si>
-  <si>
-    <t>28/12/22 (quarta-feira): Los Angeles Lakers x Miami Heat (ESPN 2 – 21h30)</t>
-  </si>
-  <si>
-    <t>30/12/22 (sexta-feira): Miami Heat x Denver Nuggets (ESPN 2 – 23h)</t>
-  </si>
-  <si>
-    <t>01/01/23 (domingo): Boston Celtics x Denver Nuggets (TNT / SporTV 2 / Gaules / Facebook da CNN Brasil – 22h)</t>
-  </si>
-  <si>
-    <t>02/01/23 (segunda-feira): Atlanta Hawks x Golden State Warriors (Band / TNT / SporTV 2 / Gaules / Facebook da CNN Brasil – 0h30)</t>
-  </si>
-  <si>
-    <t>03/01/23 (terça-feira): Washington Wizards x Milwaukee Bucks (Amazon Prime Video – 22h)</t>
-  </si>
-  <si>
-    <t>04/01/23 (quarta-feira): Milwaukee Bucks x Toronto Raptors (ESPN 2 – 21h30) / Miami Heat x Los Angeles Lakers (ESPN 2 – 0h)</t>
-  </si>
-  <si>
-    <t>05/01/23 (quinta-feira): Boston Celtics x Dallas Mavericks (Amazon Prime Video – 21h30) / Los Angeles Clippers x Denver Nuggets (Amazon Prime Video – 0h)</t>
-  </si>
-  <si>
-    <t>06/01/23 (sexta-feira): Chicago Bulls x Philadelphia 76ers (ESPN 2 – 21h30) / Miami Heat x Phoenix Suns (ESPN 2 – 0h)</t>
-  </si>
-  <si>
-    <t>07/01/23 (sábado): New Orleans Pelicans x Dallas Mavericks (Amazon Prime Video – 22h) / Orlando Magic x Golden State Warriors (ESPN 2 – 22h30)</t>
-  </si>
-  <si>
-    <t>08/01/23 (domingo): Atlanta Hawks x Los Angeles Clippers (Band / TNT / SporTV 2 / Gaules / Facebook da CNN Brasil – 23h)</t>
-  </si>
-  <si>
-    <t>09/01/23 (segunda-feira): Los Angeles Lakers x Denver Nuggets (Band / TNT / SporTV 2 / Gaules / Facebook da CNN Brasil – 23h)</t>
-  </si>
-  <si>
-    <t>10/01/23 (terça-feira): Detroit Pistons x Philadelphia 76ers (Amazon Prime Video – 21h30)</t>
-  </si>
-  <si>
-    <t>11/01/23 (quarta-feira): Milwaukee Bucks x Atlanta Hawks (ESPN 2 – 21h30) / Houston Rockets x Sacramento Kings (ESPN 2 – 0h)</t>
-  </si>
-  <si>
-    <t>12/01/23 (quinta-feira): Boston Celtics x Brooklyn Nets (Amazon Prime Video – 21h30)</t>
-  </si>
-  <si>
-    <t>13/01/23 (sexta-feira): Golden State Warriors x San Antonio Spurs (ESPN 2 – 21h30) / Denver Nuggets x Los Angeles Clippers (ESPN 2 – 0h)</t>
-  </si>
-  <si>
-    <t>14/01/23 (sábado): Milwaukee Bucks x Miami Heat (ESPN 2 – 15h) / Boston Celtics x Charlotte Hornets (Amazon Prime Video – 21h)</t>
-  </si>
-  <si>
-    <t>15/01/23 (domingo): Philadelphia 76ers x Los Angeles Lakers (Band / TNT / SporTV 2 / Gaules / Facebook da CNN Brasil – 23h30)</t>
-  </si>
-  <si>
-    <t>16/01/23 (segunda-feira): Houston Rockets x Los Angeles Lakers (Band / TNT / SporTV 2 / Gaules / Facebook da CNN Brasil – 0h30)</t>
-  </si>
-  <si>
-    <t>17/01/23 (terça-feira): Toronto Raptors x Milwaukee Bucks (Amazon Prime Video – 21h30) / Philadelphia 76ers x Los Angeles Clippers (Amazon Prime Video – 0h)</t>
-  </si>
-  <si>
-    <t>18/01/23 (quarta-feira): Atlanta Hawks x Dallas Mavericks (ESPN 2 – 21h30) / Minnesota Timberwolves x Denver Nuggets (ESPN 2 – 0h)</t>
-  </si>
-  <si>
-    <t>19/01/23 (quinta-feira): Golden State Warriors x Boston Celtics (Amazon Prime Video – 21h30) / Brooklyn Nets x Phoenix Suns (Amazon Prime Video – 0h)</t>
-  </si>
-  <si>
-    <t>20/01/23 (sexta-feira): Miami Heat x Dallas Mavericks (ESPN 2 – 21h30) / Memphis Grizzlies x Los Angeles Lakers (ESPN 2 – 0h)</t>
-  </si>
-  <si>
-    <t>21/01/23 (sábado): Milwaukee Bucks x Cleveland Cavaliers (Amazon Prime Video – 21h30)</t>
-  </si>
-  <si>
-    <t>22/01/23 (domingo): Brooklyn Nets x Golden State Warriors (TNT / SporTV 2 / Gaules / Facebook da CNN Brasil – 22h30)</t>
-  </si>
-  <si>
-    <t>23/01/23 (segunda-feira): Charlotte Hornets x Utah Jazz (Band / TNT / SporTV 2 / Gaules / Facebook da CNN Brasil – 23h)</t>
-  </si>
-  <si>
-    <t>24/01/23 (terça-feira): Boston Celtics x Miami Heat (Amazon Prime Video – 21h30) / Los Angeles Clippers x Los Angeles Lakers (Amazon Prime Video – 0h)</t>
-  </si>
-  <si>
-    <t>25/01/23 (quarta-feira): Brooklyn Nets x Philadelphia 76ers (ESPN 2 – 21h30) / Memphis Grizzlies x Golden State Warriors (ESPN 2 – 0h)</t>
-  </si>
-  <si>
-    <t>26/01/23 (quinta-feira): Chicago Bulls x Charlotte Hornets (Amazon Prime Video – 21h30) / Dallas Mavericks x Phoenix Suns (Amazon Prime Video – 0h)</t>
-  </si>
-  <si>
-    <t>27/01/23 (sexta-feira): Memphis Grizzlies x Minnesota Timberwolves (ESPN 2 – 21h30)</t>
-  </si>
-  <si>
-    <t>28/01/23 (sábado): Denver Nuggets x Philadelphia 76ers (ESPN 2 – 17h) / New York Knicks x Brooklyn Nets (ESPN 2 – 19h30) / Karim Benzema / Los Angeles Clippers x Atlanta Hawks (Amazon Prime Video – 21h30) / Los Angeles Lakers x Boston Celtics (ESPN 2 – 22h30)</t>
-  </si>
-  <si>
-    <t>30/01/23 (segunda-feira): Toronto Raptors x Phoenix Suns (Band / TNT / SporTV 2 / Gaules / Facebook da CNN Brasil – 23h)</t>
-  </si>
-  <si>
-    <t>31/01/23 (terça-feira): Los Angeles Lakers x New York Knicks (Amazon Prime Video – 21h30) / New Orleans Pelicans x Denver Nuggets (Amazon Prime Video – 0h)</t>
-  </si>
-  <si>
-    <t>01/02/23 (quarta-feira): Brooklyn Nets x Boston Celtics (ESPN 2 – 21h30) / Atlanta Hawks x Phoenix Suns (ESPN 2 – 0h)</t>
-  </si>
-  <si>
-    <t>02/02/23 (quinta-feira): Memphis Grizzlies x Cleveland Cavaliers (Amazon Prime Video – 21h30) / Los Angeles Clippers x Milwaukee Bucks (Amazon Prime Video – 0h)</t>
-  </si>
-  <si>
-    <t>04/02/23 (sábado): Los Angeles Clippers x New York Knicks (Amazon Prime Video – 21h) / Dallas Mavericks x Golden State Warriors (ESPN 2 – 22h30)</t>
-  </si>
-  <si>
-    <t>05/02/23 (domingo): Philadelphia 76ers x New York Knicks (ESPN 2 – 20h) / Denver Nuggets x Minnesota Timberwolves (TNT / SporTV 2 / Gaules / Facebook da CNN Brasil – 21h)</t>
-  </si>
-  <si>
-    <t>06/02/23 (segunda-feira): Milwaukee Bucks x Portland Trail Blazers (Band / TNT / SporTV 2 / Gaules / Facebook da CNN Brasil – 0h)</t>
-  </si>
-  <si>
-    <t>07/02/23 (terça-feira): Atlanta Hawks x New Orleans Pelicans (Amazon Prime Video – 21h30) / Minnesota Timberwolves x Denver Nuggets (Amazon Prime Video – 0h)</t>
-  </si>
-  <si>
-    <t>08/02/23 (quarta-feira): Philadelphia 76ers x Boston Celtics (ESPN 2 – 21h30) / Dallas Mavericks x Los Angeles Clippers (ESPN 2 – 0h)</t>
-  </si>
-  <si>
-    <t>09/02/23 (quinta-feira): Chicago Bulls x Brooklyn Nets (Amazon Prime Video – 21h30) / Milwaukee Bucks x Los Angeles Lakers (Amazon Prime Video – 0h)</t>
-  </si>
-  <si>
-    <t>10/02/23 (sexta-feira): Charlotte Hornets x Boston Celtics (ESPN 2 – 21h30) / Cleveland Cavaliers x New Orleans Pelicans (ESPN 2 – 0h)</t>
-  </si>
-  <si>
-    <t>11/02/23 (sábado): Chicago Bulls x Cleveland Cavaliers (Amazon Prime Video – 22h) /  Los Angeles Lakers x Golden State Warriors (ESPN 2 – 22h30)</t>
-  </si>
-  <si>
-    <t>12/02/23 (domingo): Memphis Grizzlies x Boston Celtics (ESPN 2 – 16h)</t>
-  </si>
-  <si>
-    <t>13/02/23 (segunda-feira): Washington Wizards x Golden State Warriors (Band / TNT / SporTV 2 / Gaules / Facebook da CNN Brasil – 0h)</t>
-  </si>
-  <si>
-    <t>14/02/23 (terça-feira): Boston Celtics x Milwaukee Bucks (Amazon Prime Video – 21h30) / Golden State Warriors x Los Angeles Clippers (Amazon Prime Video – 0h)</t>
-  </si>
-  <si>
-    <t>15/02/23 (quarta-feira): Miami Heat x Brooklyn Nets (ESPN 2 – 21h30) / New Orleans Pelicans x Los Angeles Lakers (ESPN 2 – 0h)</t>
-  </si>
-  <si>
-    <t>16/02/23 (quinta-feira): Milwaukee Bucks x Chicago Bulls (Amazon Prime Video – 21h30) / Los Angeles Clippers x Phoenix Suns (Amazon Prime Video – 0h)</t>
-  </si>
-  <si>
-    <t>23/02/23 (quinta-feira): Memphis Grizzlies x Philadelphia 76ers (Amazon Prime Video – 21h30) / Golden State Warriors x Los Angeles Lakers (Amazon Prime Video – 0h)</t>
-  </si>
-  <si>
-    <t>24/02/23 (sexta-feira): Miami Heat x Milwaukee Bucks (ESPN 2 – 21h30) / Brooklyn Nets x Chicago Bulls (ESPN 2 – 0h)</t>
-  </si>
-  <si>
-    <t>25/02/23 (sábado): Denver Nuggets x Memphis Grizzlies (Amazon Prime Video – 22h) / Boston Celtics x Philadelphia 76ers (ESPN 2 – 22h30)</t>
-  </si>
-  <si>
-    <t>26/02/23 (domingo): Phoenix Suns x Milwaukee Bucks (ESPN 2 – 15h) / Los Angeles Lakers x Dallas Mavericks (ESPN 2 – 17h30) / Minnesota Timberwolves x Golden State Warriors (ESPN 2 – 21h30) / Los Angeles Clippers x Denver Nuggets (ESPN 2 – 0h)</t>
-  </si>
-  <si>
-    <t>28/02/23 (terça-feira): Washington Wizards x Atlanta Hawks (Amazon Prime Video – 21h30) / Minnesota Timberwolves x Los Angeles Clippers (Amazon Prime Video – 0h)</t>
-  </si>
-  <si>
-    <t>01/03/23 (quarta-feira): Cleveland Cavaliers x Boston Celtics (ESPN 2 – 21h30) / New Orleans Pelicans x Portland Trail Blazers (ESPN 2 – 0h)</t>
-  </si>
-  <si>
-    <t>02/03/23 (quinta-feira): Philadelphia 76ers x Dallas Mavericks (Amazon Prime Video – 21h30) / Los Angeles Clippers x Golden State Warriors (Amazon Prime Video – 0h)</t>
-  </si>
-  <si>
-    <t>03/03/23 (sexta-feira): Brooklyn Nets x Boston Celtics (ESPN 2 – 21h30) / Memphis Grizzlies x Denver Nuggets (ESPN 2 – 0h)</t>
-  </si>
-  <si>
-    <t>04/03/23 (sábado): Atlanta Hawks x Miami Heat (Amazon Prime Video – 22h) / Philadelphia 76ers x Milwaukee Bucks (ESPN 2 – 22h30)</t>
-  </si>
-  <si>
-    <t>05/03/23 (domingo): Phoenix Suns x Dallas Mavericks (ESPN 2 – 15h) / Golden State Warriors x Los Angeles Lakers (ESPN 2 – 17h30) / Charlotte Hornets x Brooklyn Nets (TNT / SporTV 2 / Gaules / Facebook da CNN Brasil – 20h) / New York Knicks x Boston Celtics (ESPN 2 – 21h30) / Memphis Grizzlies x Los Angeles Clippers (ESPN 2 – 0h)</t>
-  </si>
-  <si>
-    <t>06/03/23 (segunda-feira): Toronto Raptors x Denver Nuggets (Band / TNT / SporTV 2 / Gaules / Facebook da CNN Brasil – 23h)</t>
-  </si>
-  <si>
-    <t>07/03/23 (terça-feira): Philadelphia 76ers x Minnesota Timberwolves (Amazon Prime Video – 21h30) / Memphis Grizzlies x Los Angeles Lakers (Amazon Prime Video – 0h)</t>
-  </si>
-  <si>
-    <t>08/03/23 (quarta-feira): Dallas Mavericks x New Orleans Pelicans (ESPN 2 – 21h30) / Toronto Raptors x Los Angeles Clippers (ESPN 2 – 0h)</t>
-  </si>
-  <si>
-    <t>09/03/23 (quinta-feira): Brooklyn Nets x Milwaukee Bucks (Amazon Prime Video – 21h30) / Golden State Warriors x Memphis Grizzlies (Amazon Prime Video – 0h)</t>
-  </si>
-  <si>
-    <t>10/03/23 (sexta-feira): Toronto Raptors x Los Angeles Lakers (ESPN 2 – 0h30)</t>
-  </si>
-  <si>
-    <t>11/03/23 (sábado): Dallas Mavericks x Memphis Grizzlies (Amazon Prime Video – 22h) / Milwaukee Bucks x Golden State Warriors (ESPN 2 – 22h30)</t>
-  </si>
-  <si>
-    <t>12/03/23 (domingo): New York Knicks x Los Angeles Lakers (ESPN 2 – 22h)</t>
-  </si>
-  <si>
-    <t>13/03/23 (segunda-feira): Memphis Grizzlies x Dallas Mavericks (ESPN 2 – 20h30) / Phoenix Suns x Golden State Warriors (ESPN 2 – 23h) / Milwaukee Bucks x Sacramento Kings (Band / TNT / SporTV 2 / Gaules / Facebook da CNN Brasil – 23h)</t>
-  </si>
-  <si>
-    <t>14/03/23 (terça-feira): Denver Nuggets x Toronto Raptors (Amazon Prime Video – 20h30) / Milwaukee Bucks x Phoenix Suns (Amazon Prime Video – 23h)</t>
-  </si>
-  <si>
-    <t>15/03/23 (quarta-feira): Philadelphia 76ers x Cleveland Cavaliers (ESPN 2 – 20h30) / Golden State Warriors x Los Angeles Clippers (ESPN 2 – 23h)</t>
-  </si>
-  <si>
-    <t>16/03/23 (quinta-feira): Denver Nuggets x Detroit Pistons (Amazon Prime Video – 20h) / Orlando Magic x Phoenix Suns (Amazon Prime Video – 23h)</t>
-  </si>
-  <si>
-    <t>17/03/23 (sexta-feira): Dallas Mavericks x Los Angeles Lakers (ESPN 2 – 23h30)</t>
-  </si>
-  <si>
-    <t>18/03/23 (sábado): Golden State Warriors x Memphis Grizzlies (Amazon Prime Video – 21h)</t>
-  </si>
-  <si>
-    <t>19/03/23 (domingo): Orlando Magic x Los Angeles Lakers (TNT / SporTV 2 / Gaules / Facebook da CNN Brasil – 22h30)</t>
-  </si>
-  <si>
-    <t>21/03/23 (terça-feira): Cleveland Cavaliers x Brooklyn Nets (Amazon Prime Video – 20h30) / Boston Celtics x Sacramento Kings (Amazon Prime Video – 23h)</t>
-  </si>
-  <si>
-    <t>22/03/23 (quarta-feira): Golden State Warriors x Dallas Mavericks (ESPN 2 – 20h30) / Phoenix Suns x Los Angeles Lakers (ESPN 2 – 23h)</t>
-  </si>
-  <si>
-    <t>23/03/23 (quinta-feira): New York Knicks x Orlando Magic (Amazon Prime Video – 20h) / Oklahoma City Thunder x Los Angeles Clippers (Amazon Prime Video – 23h30)</t>
-  </si>
-  <si>
-    <t>24/03/23 (sexta-feira): Philadelphia 76ers x Golden State Warriors (ESPN 2 – 23h)</t>
-  </si>
-  <si>
-    <t>25/03/23 (sábado): Brooklyn Nets x Miami Heat (Amazon Prime Video – 21h) / Milwaukee Bucks x Denver Nuggets (ESPN 2 – 22h)</t>
-  </si>
-  <si>
-    <t>26/03/23 (domingo): Minnesota Timberwolves x Golden State Warriors (TNT / SporTV 2 / Gaules / Facebook da CNN Brasil – 21h30)</t>
-  </si>
-  <si>
-    <t>27/03/23 (segunda-feira): Chicago Bulls x Los Angeles Clippers (Band / TNT / SporTV 2 / Gaules / Facebook da CNN Brasil – 23h30)</t>
-  </si>
-  <si>
-    <t>28/03/23 (terça-feira): Miami Heat x Toronto Raptors (Amazon Prime Video – 20h30) / New Orleans Pelicans x Golden State Warriors (Amazon Prime Video – 23h)</t>
-  </si>
-  <si>
-    <t>29/03/23 (quarta-feira): Dallas Mavericks x Philadelphia 76ers (ESPN 2 – 20h30) / Minnesota Timberwolves x Phoenix Suns (ESPN 2 – 23h)</t>
-  </si>
-  <si>
-    <t>30/03/23 (quinta-feira): Boston Celtics x Milwaukee Bucks (Amazon Prime Video – 20h30) / New Orleans Pelicans x Denver Nuggets (Amazon Prime Video – 23h)</t>
-  </si>
-  <si>
-    <t>31/03/23 (sexta-feira): Los Angeles Clippers x Memphis Grizzlies (ESPN 2 – 21h)</t>
-  </si>
-  <si>
-    <t>01/04/23 (sábado): Dallas Mavericks x Miami Heat (ESPN 2 – 20h30) / Los Angeles Clippers x New Orleans Pelicans (Amazon Prime Video – 21h30)</t>
-  </si>
-  <si>
-    <t>02/04/23 (domingo): Philadelphia 76ers x Milwaukee Bucks (TNT / SporTV 2 / Gaules / Facebook da CNN Brasil – 21h)</t>
-  </si>
-  <si>
-    <t>04/04/23 (terça-feira): Boston Celtics x Philadelphia 76ers (Amazon Prime Video – 21h)</t>
-  </si>
-  <si>
-    <t>05/04/23 (quarta-feira): Chicago Bulls x Milwaukee Bucks (ESPN 2 – 20h30) / Los Angeles Lakers x Los Angeles Clippers (ESPN 2 – 23h)</t>
-  </si>
-  <si>
-    <t>06/04/23 (quinta-feira): Miami Heat x Philadelphia 76ers (Amazon Prime Video – 20h30) / Denver Nuggets x Phoenix Suns (Amazon Prime Video – 23h)</t>
-  </si>
-  <si>
-    <t>07/04/23 (sexta-feira): Phoenix Suns x Los Angeles Lakers (ESPN 2 – 23h30)</t>
-  </si>
-  <si>
-    <t>08/04/23 (sábado): Denver Nuggets x Utah Jazz (ESPN 2 – 16h30) / Portland Trail Blazers x Los Angeles Clippers (Amazon Prime Video – 17h)</t>
-  </si>
-  <si>
-    <t>09/04/23 (domingo): Golden State Warriors x Portland Trail Blazers (TNT / SporTV 2 / Gaules / Facebook da CNN Brasil – 16h30)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="130">
+  <si>
+    <t>07/10 (sábado): Los Angeles Lakers x Golden State Warriors – 21h30 (Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>08/10 (domingo): Philadelphia 76ers x Boston Celtics (19h – ESPN 3)</t>
+  </si>
+  <si>
+    <t>10/10 (terça): Denver Nuggets x Phoenix Suns – 23h (Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>13/10 (sexta-feira): Miami Heat x San Antonio Spurs – 20h30 (Amazon Prime Video), Golden State Warriors x Los Angeles Lakers (23h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>15/10 (domingo): Milwaukee Bucks x Los Angeles Lakers (20h – ESPN 3), Golden State Warriors x Sacramento Kings (22h30 – ESPN 3)</t>
+  </si>
+  <si>
+    <t>17/10 (terça-feira): New York Knicks x Boston Celtics – 20h30 (Amazon Prime Video), Denver Nuggets x Los Angeles Clippers (23h30 – ESPN 2)</t>
+  </si>
+  <si>
+    <t>20/10 (sexta): Flamengo x Orlando Magic – 20h (Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>25/10 (quarta-feira): Boston Celtics x New York Knicks (20h – ESPN 2), Dallas Mavericks x San Antonio Spurs (22h30 – ESPN 2)</t>
+  </si>
+  <si>
+    <t>27/10 (sexta-feira): Miami Heat x Boston Celtics (20h30 – ESPN 2), Golden State Warriors x Sacramento Kings (23h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>24/10 (terça-feira): Los Angeles Lakers x Denver Nuggets (20h30 – Amazon Prime Video), Phoenix Suns x Golden State Warriors (23h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>26/10 (quinta-feira): Philadelphia 76ers x Milwaukee Bucks (20h30 – Amazon Prime Video), Phoenix Suns x Los Angeles Lakers (23h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>28/10 (sábado): New York Knicks x New Orleans Pelicans (20h – Amazon Prime Video), Miami Heat x Minnesota Timberwolves (21h – ESPN 2), Utah Jazz x Phoenix Suns (23h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>29/10 (domingo): Denver Nuggets x Oklahoma City Thunder (16h30 – Amazon Prime Video), Los Angeles Lakers x Sacramento Kings (22h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>31/10 (terça-feira): New York Knicks x Cleveland Cavaliers (20h30 – Amazon Prime Video), San Antonio Spurs x Phoenix Suns (23h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>01/11 (quarta-feira): New Orleans Pelicans x Oklahoma City Thunder (20h30 – ESPN 2), Los Angeles Clippers x Los Angeles Lakers (23h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>03/11 (sexta-feira): New York Knicks x Milwaukee Bucks (20h30 – ESPN 2), Dallas Mavericks x Denver Nuggets (23h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>04/11 (sábado): Phoenix Suns x Philadelphia 76ers (14h – Amazon Prime Video), Los Angeles Lakers x Orlando Magic (20h – ESPN 2), Chicago Bulls x Denver Nuggets (22h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>05/11 (domingo): Toronto Raptors x San Antonio Spurs (17h30 – Amazon Prime Video), Golden State Warriors x Cleveland Cavaliers (20h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>08/11 (quarta-feira): San Antonio Spurs x New York Knicks (21h30 – ESPN 2), Golden State Warriors x Denver Nuggets (0h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>10/11 (sexta-feira): Brooklyn Nets x Boston Celtics (21h30 – ESPN 2), Los Angeles Lakers x Phoenix Suns (0h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>11/11 (sábado): Miami Heat x Atlanta Hawks (21h30 – Amazon Prime Video), Cleveland Cavaliers x Golden State Warriors (22h30 – ESPN 2)</t>
+  </si>
+  <si>
+    <t>12/11 (domingo): Memphis Grizzlies x Los Angeles Clippers (17h30 – Amazon Prime Video), Miami Heat x San Antonio Spurs (21h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>14/11 (terça-feira): San Antonio Spurs x Oklahoma City Thunder (21h30 – Amazon Prime Video), Los Angeles Clippers x Denver Nuggets (0h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>15/11 (quarta-feira): Boston Celtics x Philadelphia 76ers (21h30 – ESPN 2), Sacramento Kings x Los Angeles Lakers (0h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>17/11 (sexta-feira): Sacramento Kings x San Antonio Spurs (21h30 – ESPN 2), Phoenix Suns x Utah Jazz (0h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>18/11 (sábado): Dallas Mavericks x Milwaukee Bucks (22h – Amazon Prime Video), Memphis Grizzlies x San Antonio Spurs (22h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>19/11 (domingo): Philadelphia 76ers x Brooklyn Nets (17h – Amazon Prime Video), Sacramento Kings x Dallas Mavericks (21h30 – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>21/11 (terça-feira): Cleveland Cavaliers x Philadelphia 76ers (21h30 – Amazon Prime Video), Utah Jazz x Los Angeles Lakers (0h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>22/11 (quarta-feira): Milwaukee Bucks x Boston Celtics (21h30 – ESPN 2), Golden State Warriors x Phoenix Suns (0h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>24/11 (sexta-feira): Miami Heat x New York Knicks (21h30 – ESPN 2), San Antonio Spurs x Golden State Warriors (0h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>25/11 (sábado): Philadelphia 76ers x Oklahoma City Thunder (19h – Amazon Prime Video), Los Angeles Lakers x Cleveland Cavaliers (21h30 – Amazon Prime Video), Dallas Mavericks x Los Angeles Clippers (0h30 – ESPN 2)</t>
+  </si>
+  <si>
+    <t>26/11 (domingo): Portland Trail Blazers x Milwaukee Bucks (17h30 – Amazon Prime Video), Phoenix Suns x New York Knicks (20h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>28/11 (terça-feira): Milwaukee Bucks x Miami Heat (21h30 – Amazon Prime Video), Golden State Warriors x Sacramento Kings (0h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>29/11 (quarta-feira): Los Angeles Clippers x Sacramento Kings (0h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>01/12 (sexta-feira): Memphis Grizzlies x Dallas Mavericks (21h30 – ESPN 2), Denver Nuggets x Phoenix Suns (0h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>02/12 (sábado): Golden State Warriors x Los Angeles Clippers (18h – Amazon Prime Video), Oklahoma City Thunder x Dallas Mavericks (23h – Amazon Prime Video), Memphis Grizzlies x Phoenix Suns (23h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>12/12 (terça-feira): Los Angeles Lakers x Dallas Mavericks (21h30 – Amazon Prime Video), Golden State Warriors x Phoenix Suns (0h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>13/12 (quarta-feira): Los Angeles Lakers x San Antonio Spurs (22h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>15/12 (sexta-feira): Los Angeles Lakers x San Antonio Spurs (21h30 – ESPN 2), New York Knicks x Phoenix Suns (0h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>16/12 (sábado): Detroit Pistons x Milwaukee Bucks (20h – Amazon Prime Video), Chicago Bulls x Miami Heat (22h – ESPN 2), Brooklyn Nets x Golden State Warriors (22h30 – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>17/12 (domingo): New Orleans Pelicans x San Antonio Spurs (17h30 – Amazon Prime Video), Houston Rockets x Milwaukee Bucks (21h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>19/12 (terça-feira): Memphis Grizzlies x New Orleans Pelicans (21h30 – Amazon Prime Video), Boston Celtics x Golden State Warriors (0h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>20/12 (quarta-feira): Boston Celtics x Sacramento Kings (0h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>22/12 (sexta-feira): Washington Wizards x Golden State Warriors (23h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>23/12 (sábado): Milwaukee Bucks x New York Knicks (14h30 – Amazon Prime Video), Boston Celtics x Los Angeles Clippers (17h30 – Amazon Prime Video), San Antonio Spurs x Dallas Mavericks (22h30 – ESPN 2)</t>
+  </si>
+  <si>
+    <t>25/12 (segunda-feira): Milwaukee Bucks x New York Knicks (14h – ESPN 2), Golden State Warriors x Denver Nuggets (16h30 – ESPN 2), Boston Celtics x Los Angeles Lakers (19h – ESPN 2), Philadelphia 76ers x Miami Heat (22h – ESPN 2), Dallas Mavericks x Phoenix Suns (0h30 – ESPN 2)</t>
+  </si>
+  <si>
+    <t>27/12 (quarta-feira): New York Knicks x Oklahoma City Thunder (22h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>29/12 (sexta-feira): Milwaukee Bucks x Cleveland Cavaliers (21h30 – ESPN 2)</t>
+  </si>
+  <si>
+    <t>30/12 (sábado): Miami Heat x Utah Jazz (19h – ESPN 2), Dallas Mavericks x Golden State Warriors (22h30 – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>31/12 (domingo): Los Angeles Lakers x New Orleans Pelicans (21h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>03/01 (quarta-feira): Chicago Bulls x New York Knicks (21h30 – ESPN 2), Miami Heat x Los Angeles Lakers (0h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>04/01 (quinta-feira): Milwaukee Bucks x San Antonio Spurs (21h30 – Amazon Prime Video), Denver Nuggets x Golden State Warriors (0h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>05/01 (sexta-feira): New York Knicks x Philadelphia 76ers (21h30 – ESPN 2), Memphis Grizzlies x Los Angeles Lakers (0h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>06/01 (sábado): Boston Celtics x Indiana Pacers (21h – Amazon Prime Video), Utah Jazz x Philadelphia 76ers (21h30 – ESPN 2)</t>
+  </si>
+  <si>
+    <t>07/01 (domingo): San Antonio Spurs x Cleveland Cavaliers (15h – Amazon Prime Video), Memphis Grizzlies x Phoenix Suns (22h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>10/01 (quarta-feira): Philadelphia 76ers x Atlanta Hawks (21h30 – ESPN 2), New Orleans Pelicans x Golden State Warriors (0h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>11/01 (quinta-feira): Boston Celtics x Milwaukee Bucks (21h30 – Amazon Prime Video), Phoenix Suns x Los Angeles Lakers (0h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>12/01 (sexta-feira): Houston Rockets x Detroit Pistons (21h30 – ESPN 2), Charlotte Hornets x San Antonio Spurs (0h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>13/01 (sábado): Golden State Warriors x Milwaukee Bucks (22h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>14/01 (domingo): Indiana Pacers x Denver Nuggets (17h30 – Amazon Prime Video), Sacramento Kings x Milwaukee Bucks (21h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>15/01 (segunda-feira): San Antonio Spurs x Atlanta Hawks (17h30 – Amazon Prime Video), Golden State Warriors x Memphis Grizzlies (20h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>16/01 (terça-feira): Denver Nuggets x Philadelphia 76ers (21h30 – Amazon Prime Video), Oklahoma City Thunder x Los Angeles Clippers (0h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>17/01 (quarta-feira): Milwaukee Bucks x Cleveland Cavaliers (21h30 – ESPN 2), Dallas Mavericks x Los Angeles Lakers (0h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>18/01 (quinta-feira): Chicago Bulls x Toronto Raptors (21h30 – Amazon Prime Video), Memphis Grizzlies x Minnesota Timberwolves (0h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>19/01 (sexta-feira): Denver Nuggets x Boston Celtics (21h30 – ESPN 2), Dallas Mavericks x Golden State Warriors (0h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>20/01 (sábado): Milwaukee Bucks x Detroit Pistons (17h – Amazon Prime Video), San Antonio Spurs x Washington Wizards (21h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>21/01 (domingo): Indiana Pacers x Phoenix Suns (22h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>23/01 (terça-feira): New York Knicks x Brooklyn Nets (21h30 – Amazon Prime Video), Los Angeles Lakers x Los Angeles Clippers (0h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>24/01 (quarta-feira): Oklahoma City Thunder x San Antonio Spurs (21h30 – ESPN 2), Phoenix Suns x Dallas Mavericks (0h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>25/01 (quinta-feira): Boston Celtics x Miami Heat (21h30 – Amazon Prime Video), Sacramento Kings x Golden State Warriors (0h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>26/01 (sexta-feira): Dallas Mavericks x Atlanta Hawks (21h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>27/01 (sábado): Miami Heat x New York Knicks (17h – ESPN 2), Philadelphia 76ers x Denver Nuggets (19h30 – ESPN 2), Los Angeles Lakers x Golden State Warriors (22h30 – ESPN 2), Minnesota Timberwolves x San Antonio Spurs (22h30 – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>28/01 (domingo): Oklahoma City Thunder x Detroit Pistons (20h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>30/01 (terça-feira): Indiana Pacers x Boston Celtics (21h30 – Amazon Prime Video), Philadelphia 76ers x Golden State Warriors (0h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>31/01 (quarta-feira): Phoenix Suns x Brooklyn Nets (21h30 – ESPN 2), Denver Nuggets x Oklahoma City Thunder (0h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>01/02 (quinta-feira): Los Angeles Lakers x Boston Celtics (21h30 – Amazon Prime Video), Cleveland Cavaliers x Memphis Grizzlies (0h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>02/02 (sexta-feira): Golden State Warriors x Memphis Grizzlies (22h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>03/02 (sábado): Los Angeles Lakers x New York Knicks (22h30 – ESPN 2), Milwaukee Bucks x Dallas Mavericks (22h30 – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>04/02 (domingo): Memphis Grizzlies x Boston Celtics (20h – ESPN 2), Los Angeles Clippers x Miami Heat (20h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>06/02 (terça-feira): Dallas Mavericks x Brooklyn Nets (21h30 – Amazon Prime Video), Milwaukee Bucks x Phoenix Suns (0h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>07/02 (quarta-feira): Atlanta Hawks x Boston Celtics (21h30 – ESPN 2), New Orleans Pelicans x Los Angeles Clippers (0h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>08/02 (quinta-feira): Dallas Mavericks x New York Knicks (21h30 – Amazon Prime Video), Denver Nuggets x Los Angeles Lakers (0h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>09/02 (sexta-feira): New Orleans Pelicans x Los Angeles Lakers (0h30 – ESPN 2)</t>
+  </si>
+  <si>
+    <t>10/02 (sábado): Oklahoma City Thunder x Dallas Mavericks (17h – Amazon Prime Video), Phoenix Suns x Golden State Warriors (22h30 – ESPN 2)</t>
+  </si>
+  <si>
+    <t>11/02 (domingo): Boston Celtics x Miami Heat (16h – ESPN 2), Sacramento Kings x Oklahoma City Thunder (17h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>13/02 (terça-feira): Oklahoma City Thunder x Orlando Magic (21h30 – Amazon Prime Video), Sacramento Kings x Phoenix Suns (0h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>14/02 (quarta-feira): Chicago Bulls x Cleveland Cavaliers (21h30 – ESPN 2), Los Angeles Clippers x Golden State Warriors (0h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>15/02 (quinta-feira): Milwaukee Bucks x Memphis Grizzlies (22h30 – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>22/02 (quinta-feira): Phoenix Suns x Dallas Mavericks (21h30 – Amazon Prime Video), Los Angeles Lakers x Golden State Warriors (0h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>23/02 (sexta-feira): Cleveland Cavaliers x Philadelphia 76ers (21h30 – ESPN 2), Miami Heat x New Orleans Pelicans (0h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>24/02 (sábado):Brooklyn Nets x Minnesota Timberwolves (22h – Amazon Prime Video), Boston Celtics x New York Knicks (22h30 – ESPN 2)</t>
+  </si>
+  <si>
+    <t>25/02 (domingo): Milwaukee Bucks x Philadelphia 76ers (15h – ESPN 2), Los Angeles Lakers x Phoenix Suns (17h30 – ESPN 2), Denver Nuggets x Golden State Warriors (21h – ESPN 2), San Antonio Spurs x Utah Jazz (22h – Amazon Prime Video), Sacramento Kings x Los Angeles Clippers (23h30 – ESPN 2)</t>
+  </si>
+  <si>
+    <t>27/02 (terça-feira): Philadelphia 76ers x Boston Celtics (21h30 – Amazon Prime Video), Miami Heat x Portland Trail Blazers (0h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>28/02 (quarta-feira): Memphis Grizzlies x Minnesota Timberwolves (21h30 – ESPN 2), Los Angeles Lakers x Los Angeles Clippers (0h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>29/02 (quinta-feira): Golden State Warriors x New York Knicks (21h30 – Amazon Prime Video), Miami Heat x Denver Nuggets (0h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>01/03 (sexta-feira): Dallas Mavericks x Boston Celtics (21h30 – ESPN 2), Milwaukee Bucks x Chicago Bulls (0h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>02/03 (sábado): Utah Jazz x Miami Heat (19h – Amazon Prime Video), Denver Nuggets x Los Angeles Lakers (22h30 – ESPN 2)</t>
+  </si>
+  <si>
+    <t>03/03 (domingo): Philadelphia 76ers x Dallas Mavericks (15h – ESPN 2), Golden State Warriors x Boston Celtics (17h30 – ESPN 2),Los Angeles Clippers x Minnesota Timberwolves (17h30 – Amazon Prime Video), New York Knicks x Cleveland Cavaliers (21h – ESPN 2), Oklahoma City Thunder x Phoenix Suns (23h30 – ESPN 2)</t>
+  </si>
+  <si>
+    <t>05/03 (terça-feira): Atlanta Hawks x New York Knicks (21h30 – Amazon Prime Video), Phoenix Suns x Denver Nuggets (0h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>06/03 (quarta-feira): Memphis Grizzlies x Philadelphia 76ers (20h30 – ESPN 2), Milwaukee Bucks x Golden State Warriors (23h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>07/03 (quinta-feira): Miami Heat x Dallas Mavericks (21h30 – Amazon Prime Video), Boston Celtics x Denver Nuggets (0h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>08/03 (sexta-feira): Atlanta Hawks x Memphis Grizzlies (21h30 – ESPN 2), Milwaukee Bucks x Los Angeles Lakers (0h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>09/03 (sábado): Boston Celtics x Phoenix Suns (22h30 – ESPN 2), San Antonio Spurs x Golden State Warriors (22h30 – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>10/03 (domingo): Philadelphia 76ers x New York Knicks (19h – Amazon Prime Video), Brooklyn Nets x Cleveland Cavaliers (20h – ESPN 2), Minnesota Timberwolves x Los Angeles Lakers (22h30 – ESPN 2)</t>
+  </si>
+  <si>
+    <t>12/03 (terça-feira): Philadelphia 76ers x New York Knicks (20h30 – Amazon Prime Video), Minnesota Timberwolves x Los Angeles Clippers (23h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>13/03 (quarta-feira): Denver Nuggets x Miami Heat (20h30 – ESPN 2)</t>
+  </si>
+  <si>
+    <t>14/03 (quinta-feira): Phoenix Suns x Boston Celtics (20h30 – Amazon Prime Video), Dallas Mavericks x Oklahoma City Thunder (23h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>15/03 (sexta-feira): Denver Nuggets x San Antonio Spurs (21h30 – ESPN 2)</t>
+  </si>
+  <si>
+    <t>16/03 (sábado): Golden State Warriors x Los Angeles Lakers (21h30 – ESPN 2), New York Knicks x Sacramento Kings (23h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>17/03 (domingo): Phoenix Suns x Milwaukee Bucks (14h – ESPN 2), Denver Nuggets x Dallas Mavericks (16h30 – ESPN 2), Brooklyn Nets x San Antonio Spurs (20h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>18/03 (segunda-feira): Miami Heat x Philadelphia 76ers (20h30 – ESPN 2), New York Knicks x Golden State Warriors (23h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>20/03 (quarta-feira): Milwaukee Bucks x Boston Celtics (20h30 – ESPN 2), Memphis Grizzlies x Golden State Warriors (23h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>23/03 (sábado): Phoenix Suns x San Antonio Spurs (21h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>24/03 (domingo): Golden State Warriors x Minnesota Timberwolves (20h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>26/03 (terça-feira): Los Angeles Lakers x Milwaukee Bucks (20h30 – Amazon Prime Video), Dallas Mavericks x Sacramento Kings (23h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>27/03 (quarta-feira): Los Angeles Clippers x Philadelphia 76ers (20h30 – ESPN 2), Phoenix Suns x Denver Nuggets (23h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>29/03 (sexta-feira): Dallas Mavericks x Sacramento Kings (23h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>30/03 (sábado): Boston Celtics x New Orleans Pelicans (18 – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>31/03 (domingo): Cleveland Cavaliers x Denver Nuggets (16h30 – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>02/04 (terça-feira): Golden State Warriors x Dallas Mavericks (20h30 – ESPN 2), Los Angeles Clippers x Sacramento Kings (23h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>03/04 (quarta-feira): Memphis Grizzlies x Milwaukee Bucks (20h30 – ESPN 2), Cleveland Cavaliers x Phoenix Suns (23h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>04/04 (quinta-feira): Philadelphia 76ers x Miami Heat (20h30 – Amazon Prime Video), Denver Nuggets x Los Angeles Clippers (23h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>05/04 (sexta-feira): Sacramento Kings x Boston Celtics (20h30 – ESPN 2)</t>
+  </si>
+  <si>
+    <t>06/04 (sábado): Philadelphia 76ers x Memphis Grizzlies (21h – Amazon Prime Video), Atlanta Hawks x Denver Nuggets (22h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>07/04 (domingo): New York Knicks x Milwaukee Bucks (20h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>09/04 (terça-feira): Boston Celtics x Milwaukee Bucks (20h30 – Amazon Prime Video), Golden State Warriors x Los Angeles Lakers (23h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>10/04 (quarta-feira): Dallas Mavericks x Miami Heat (20h30 – ESPN 2), Minnesota Timberwolves x Denver Nuggets (23h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>11/04 (quinta-feira): New York Knicks x Boston Celtics (20h30 – Amazon Prime Video), New Orleans Pelicans x Sacramento Kings (23h – Amazon Prime Video)</t>
+  </si>
+  <si>
+    <t>12/04 (sexta-feira): Los Angeles Lakers x Memphis Grizzlies (21h – ESPN 2)</t>
+  </si>
+  <si>
+    <t>14/04 (domingo): Los Angeles Lakers x New Orleans Pelicans (16h30 – Amazon Prime Video)</t>
   </si>
 </sst>
 </file>
@@ -507,8 +461,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -789,11 +744,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A149"/>
+  <dimension ref="A1:A130"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="12" max="12" width="11" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1391,153 +1351,58 @@
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A120" t="s">
+      <c r="A120" s="1" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A121" t="s">
+      <c r="A121" s="1" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A122" t="s">
+      <c r="A122" s="1" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A123" t="s">
+      <c r="A123" s="1" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A124" t="s">
+      <c r="A124" s="1" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A125" t="s">
+      <c r="A125" s="1" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A126" t="s">
+      <c r="A126" s="1" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A127" t="s">
+      <c r="A127" s="1" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A128" t="s">
+      <c r="A128" s="1" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A129" t="s">
+      <c r="A129" s="1" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A130" t="s">
+      <c r="A130" s="1" t="s">
         <v>129</v>
-      </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A131" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A132" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A133" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A134" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A135" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A136" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A137" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A138" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A139" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A140" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A141" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A142" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A143" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A144" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A145" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A146" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A147" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A148" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A149" t="s">
-        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>